<commit_message>
Add Erlotinib bio rep 3 and 1 datasets
</commit_message>
<xml_diff>
--- a/Datasets/MTT_Erlotinib bio rep 3.xlsx
+++ b/Datasets/MTT_Erlotinib bio rep 3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0117675\Documents\DOCTORAAT\Resultaten\WP1 - Aa mutants\Stable ARK1 expressing mutants\Compound treatment\Sophie\Combinaties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/myluong_vuong_kuleuven_be/Documents/PhD in KU Leuven/Projects/Side projects/Cancer Invitro/Report_Oncology_MLV/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3614EF9-4B5C-4082-BAF0-CD54E51253E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D3614EF9-4B5C-4082-BAF0-CD54E51253E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CE791D1-2DD5-47F7-8933-07DBFE5457F0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A8AEB0EA-8269-45DA-8308-9EA05609BCA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A8AEB0EA-8269-45DA-8308-9EA05609BCA6}"/>
   </bookViews>
   <sheets>
     <sheet name="WT" sheetId="2" r:id="rId1"/>
@@ -433,13 +433,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95593D7-FC6C-48C2-AAA9-DD5F29425F0D}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1051,13 +1051,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2BA38FD-6D55-4625-BDF4-F2C79E2B084F}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1360,304 +1363,304 @@
         <v>91.71730092740647</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <f>175/3</f>
         <v>58.333333333333336</v>
       </c>
-      <c r="C13" s="2">
-        <f>B13/3</f>
+      <c r="C14" s="2">
+        <f>B14/3</f>
         <v>19.444444444444446</v>
       </c>
-      <c r="D13" s="2">
-        <f t="shared" ref="D13:G13" si="2">C13/3</f>
+      <c r="D14" s="2">
+        <f t="shared" ref="D14:G14" si="2">C14/3</f>
         <v>6.4814814814814818</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="2">
         <f t="shared" si="2"/>
         <v>2.1604938271604941</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
         <f t="shared" si="2"/>
         <v>0.72016460905349799</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G14" s="2">
         <f t="shared" si="2"/>
         <v>0.24005486968449932</v>
       </c>
-      <c r="H13" s="2">
-        <f>G13/3</f>
+      <c r="H14" s="2">
+        <f>G14/3</f>
         <v>8.0018289894833103E-2</v>
       </c>
-      <c r="I13" s="2">
-        <f>H13/3</f>
+      <c r="I14" s="2">
+        <f>H14/3</f>
         <v>2.66727632982777E-2</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>33.936843594186499</v>
-      </c>
-      <c r="C14">
-        <v>35.475087520775133</v>
-      </c>
-      <c r="D14">
-        <v>38.403055270695567</v>
-      </c>
-      <c r="E14">
-        <v>87.319212136214162</v>
-      </c>
-      <c r="F14">
-        <v>60.235510449450125</v>
-      </c>
-      <c r="G14">
-        <v>59.461084196753774</v>
-      </c>
-      <c r="H14">
-        <v>72.838502068672867</v>
-      </c>
-      <c r="I14">
-        <v>74.047880052335643</v>
-      </c>
-      <c r="J14">
-        <v>60.362813395098833</v>
-      </c>
-      <c r="K14">
-        <v>102.00148520103258</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>32.228862406732908</v>
+        <v>33.936843594186499</v>
       </c>
       <c r="C15">
-        <v>39.580607517946177</v>
+        <v>35.475087520775133</v>
       </c>
       <c r="D15">
-        <v>48.916156865518587</v>
+        <v>38.403055270695567</v>
       </c>
       <c r="E15">
-        <v>101.87418225538384</v>
+        <v>87.319212136214162</v>
       </c>
       <c r="F15">
-        <v>42.975352735245238</v>
+        <v>60.235510449450125</v>
       </c>
       <c r="G15">
-        <v>79.882598394568404</v>
+        <v>59.461084196753774</v>
       </c>
       <c r="H15">
-        <v>95.148343293610111</v>
+        <v>72.838502068672867</v>
       </c>
       <c r="I15">
-        <v>138.67534212666644</v>
+        <v>74.047880052335643</v>
       </c>
       <c r="J15">
-        <v>98.72343435057816</v>
+        <v>60.362813395098833</v>
       </c>
       <c r="K15">
-        <v>128.62901799922204</v>
+        <v>102.00148520103258</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>32.228862406732908</v>
+      </c>
+      <c r="C16">
+        <v>39.580607517946177</v>
+      </c>
+      <c r="D16">
+        <v>48.916156865518587</v>
+      </c>
+      <c r="E16">
+        <v>101.87418225538384</v>
+      </c>
+      <c r="F16">
+        <v>42.975352735245238</v>
+      </c>
+      <c r="G16">
+        <v>79.882598394568404</v>
+      </c>
+      <c r="H16">
+        <v>95.148343293610111</v>
+      </c>
+      <c r="I16">
+        <v>138.67534212666644</v>
+      </c>
+      <c r="J16">
+        <v>98.72343435057816</v>
+      </c>
+      <c r="K16">
+        <v>128.62901799922204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>33.310937444746983</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>41.734149015170267</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>62.728526468404119</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>102.18183104070158</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>95.042257505569509</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>100.21924396195057</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>114.29682803493758</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>121.77587609179956</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>83.266735033063412</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>69.369496799745406</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="2">
         <f>175/3</f>
         <v>58.333333333333336</v>
       </c>
-      <c r="C18" s="2">
-        <f>B18/3</f>
+      <c r="C19" s="2">
+        <f>B19/3</f>
         <v>19.444444444444446</v>
       </c>
-      <c r="D18" s="2">
-        <f t="shared" ref="D18:G18" si="3">C18/3</f>
+      <c r="D19" s="2">
+        <f t="shared" ref="D19:G19" si="3">C19/3</f>
         <v>6.4814814814814818</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="2">
         <f t="shared" si="3"/>
         <v>2.1604938271604941</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <f t="shared" si="3"/>
         <v>0.72016460905349799</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G19" s="2">
         <f t="shared" si="3"/>
         <v>0.24005486968449932</v>
       </c>
-      <c r="H18" s="2">
-        <f>G18/3</f>
+      <c r="H19" s="2">
+        <f>G19/3</f>
         <v>8.0018289894833103E-2</v>
       </c>
-      <c r="I18" s="2">
-        <f>H18/3</f>
+      <c r="I19" s="2">
+        <f>H19/3</f>
         <v>2.66727632982777E-2</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <v>34.782608695652172</v>
-      </c>
-      <c r="C19">
-        <v>76.466037443911489</v>
-      </c>
-      <c r="D19">
-        <v>123.2863995048739</v>
-      </c>
-      <c r="E19">
-        <v>165.88271700448709</v>
-      </c>
-      <c r="F19">
-        <v>136.06684202382795</v>
-      </c>
-      <c r="G19">
-        <v>190.88658517716232</v>
-      </c>
-      <c r="H19">
-        <v>144.05075042549899</v>
-      </c>
-      <c r="I19">
-        <v>152.66903914590748</v>
-      </c>
-      <c r="J19">
-        <v>129.1660219712208</v>
-      </c>
-      <c r="K19">
-        <v>100.13925421630823</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20">
-        <v>37.428438805508279</v>
+        <v>34.782608695652172</v>
       </c>
       <c r="C20">
-        <v>70.462633451957302</v>
+        <v>76.466037443911489</v>
       </c>
       <c r="D20">
-        <v>144.94816648615193</v>
+        <v>123.2863995048739</v>
       </c>
       <c r="E20">
-        <v>181.21615348909177</v>
+        <v>165.88271700448709</v>
       </c>
       <c r="F20">
-        <v>117.46866780133065</v>
+        <v>136.06684202382795</v>
       </c>
       <c r="G20">
-        <v>180.643663933158</v>
+        <v>190.88658517716232</v>
       </c>
       <c r="H20">
-        <v>128.53164165248336</v>
+        <v>144.05075042549899</v>
       </c>
       <c r="I20">
-        <v>122.35803806281911</v>
+        <v>152.66903914590748</v>
       </c>
       <c r="J20">
-        <v>114.62169271236269</v>
+        <v>129.1660219712208</v>
       </c>
       <c r="K20">
-        <v>95.698591985146237</v>
+        <v>100.13925421630823</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>37.428438805508279</v>
+      </c>
+      <c r="C21">
+        <v>70.462633451957302</v>
+      </c>
+      <c r="D21">
+        <v>144.94816648615193</v>
+      </c>
+      <c r="E21">
+        <v>181.21615348909177</v>
+      </c>
+      <c r="F21">
+        <v>117.46866780133065</v>
+      </c>
+      <c r="G21">
+        <v>180.643663933158</v>
+      </c>
+      <c r="H21">
+        <v>128.53164165248336</v>
+      </c>
+      <c r="I21">
+        <v>122.35803806281911</v>
+      </c>
+      <c r="J21">
+        <v>114.62169271236269</v>
+      </c>
+      <c r="K21">
+        <v>95.698591985146237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>43.896023518489869</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>57.929753984217861</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>92.356490793749032</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>96.53411728299551</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>91.319820516787871</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>96.302026922481815</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <v>95.327247408324311</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <v>104.25498994275104</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <v>98.530094383413285</v>
       </c>
-      <c r="K21">
+      <c r="K22">
         <v>104.16215379854556</v>
       </c>
     </row>

</xml_diff>